<commit_message>
LoginTest update + allure-results
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428E9B63-15CD-44A0-B5E4-185D64AF6E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E96C18-6AD9-472C-8248-F8A87D9CA13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="188">
   <si>
     <t>ID</t>
   </si>
@@ -965,7 +965,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1038,6 +1038,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="32">
     <border>
@@ -1460,7 +1466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1771,6 +1777,48 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1780,53 +1828,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2111,8 +2120,8 @@
   <dimension ref="A1:K176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2162,11 +2171,11 @@
       <c r="J1" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="K1" s="113" t="s">
+      <c r="K1" s="108" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="61" t="s">
         <v>9</v>
       </c>
@@ -2191,9 +2200,9 @@
       <c r="J2" s="102" t="s">
         <v>183</v>
       </c>
-      <c r="K2" s="114"/>
-    </row>
-    <row r="3" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K2" s="109"/>
+    </row>
+    <row r="3" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>10</v>
       </c>
@@ -2218,7 +2227,7 @@
       <c r="J3" s="103" t="s">
         <v>183</v>
       </c>
-      <c r="K3" s="115"/>
+      <c r="K3" s="110"/>
     </row>
     <row r="4" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="100" t="s">
@@ -2244,10 +2253,10 @@
         <v>24</v>
       </c>
       <c r="I4" s="86"/>
-      <c r="J4" s="104" t="s">
+      <c r="J4" s="118" t="s">
         <v>182</v>
       </c>
-      <c r="K4" s="117" t="s">
+      <c r="K4" s="112" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2277,8 +2286,8 @@
       <c r="I5" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="105"/>
-      <c r="K5" s="116"/>
+      <c r="J5" s="119"/>
+      <c r="K5" s="111"/>
     </row>
     <row r="6" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="54" t="s">
@@ -2297,7 +2306,7 @@
       <c r="F6" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="122" t="s">
+      <c r="G6" s="117" t="s">
         <v>36</v>
       </c>
       <c r="H6" s="44" t="s">
@@ -2306,8 +2315,8 @@
       <c r="I6" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="105"/>
-      <c r="K6" s="117" t="s">
+      <c r="J6" s="119"/>
+      <c r="K6" s="112" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2337,8 +2346,8 @@
       <c r="I7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="105"/>
-      <c r="K7" s="117" t="s">
+      <c r="J7" s="119"/>
+      <c r="K7" s="112" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2366,8 +2375,8 @@
         <v>24</v>
       </c>
       <c r="I8" s="87"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="117" t="s">
+      <c r="J8" s="119"/>
+      <c r="K8" s="112" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2395,8 +2404,8 @@
         <v>24</v>
       </c>
       <c r="I9" s="87"/>
-      <c r="J9" s="105"/>
-      <c r="K9" s="117" t="s">
+      <c r="J9" s="119"/>
+      <c r="K9" s="112" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2426,8 +2435,8 @@
       <c r="I10" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="105"/>
-      <c r="K10" s="116"/>
+      <c r="J10" s="119"/>
+      <c r="K10" s="111"/>
     </row>
     <row r="11" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="57" t="s">
@@ -2453,8 +2462,8 @@
         <v>53</v>
       </c>
       <c r="I11" s="88"/>
-      <c r="J11" s="106"/>
-      <c r="K11" s="117" t="s">
+      <c r="J11" s="120"/>
+      <c r="K11" s="112" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2462,7 +2471,7 @@
       <c r="A12" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="119" t="s">
+      <c r="B12" s="114" t="s">
         <v>186</v>
       </c>
       <c r="C12" s="59"/>
@@ -2472,18 +2481,18 @@
       <c r="E12" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="120" t="s">
+      <c r="F12" s="115" t="s">
         <v>187</v>
       </c>
-      <c r="G12" s="121" t="s">
+      <c r="G12" s="116" t="s">
         <v>34</v>
       </c>
       <c r="H12" s="60" t="s">
         <v>53</v>
       </c>
       <c r="I12" s="88"/>
-      <c r="J12" s="118"/>
-      <c r="K12" s="117" t="s">
+      <c r="J12" s="113"/>
+      <c r="K12" s="112" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2514,7 +2523,7 @@
       <c r="J13" s="102" t="s">
         <v>182</v>
       </c>
-      <c r="K13" s="116"/>
+      <c r="K13" s="123"/>
     </row>
     <row r="14" spans="1:11" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
@@ -2543,7 +2552,7 @@
       <c r="J14" s="103" t="s">
         <v>183</v>
       </c>
-      <c r="K14" s="116"/>
+      <c r="K14" s="111"/>
     </row>
     <row r="15" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="36" t="s">
@@ -2570,7 +2579,7 @@
       <c r="J15" s="102" t="s">
         <v>182</v>
       </c>
-      <c r="K15" s="116"/>
+      <c r="K15" s="123"/>
     </row>
     <row r="16" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="40" t="s">
@@ -2594,10 +2603,12 @@
       </c>
       <c r="H16" s="44"/>
       <c r="I16" s="87"/>
-      <c r="J16" s="107" t="s">
+      <c r="J16" s="104" t="s">
         <v>182</v>
       </c>
-      <c r="K16" s="116"/>
+      <c r="K16" s="112" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="17" spans="1:11" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="40" t="s">
@@ -2623,10 +2634,10 @@
       <c r="I17" s="89" t="s">
         <v>77</v>
       </c>
-      <c r="J17" s="107" t="s">
+      <c r="J17" s="104" t="s">
         <v>183</v>
       </c>
-      <c r="K17" s="116"/>
+      <c r="K17" s="111"/>
     </row>
     <row r="18" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="40" t="s">
@@ -2650,10 +2661,10 @@
       </c>
       <c r="H18" s="44"/>
       <c r="I18" s="89"/>
-      <c r="J18" s="107" t="s">
+      <c r="J18" s="104" t="s">
         <v>183</v>
       </c>
-      <c r="K18" s="116"/>
+      <c r="K18" s="111"/>
     </row>
     <row r="19" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="45" t="s">
@@ -2680,7 +2691,9 @@
       <c r="J19" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="K19" s="116"/>
+      <c r="K19" s="112" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="20" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
@@ -2704,10 +2717,12 @@
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="84"/>
-      <c r="J20" s="108" t="s">
+      <c r="J20" s="105" t="s">
         <v>182</v>
       </c>
-      <c r="K20" s="116"/>
+      <c r="K20" s="112" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
@@ -2731,10 +2746,12 @@
       </c>
       <c r="H21" s="22"/>
       <c r="I21" s="91"/>
-      <c r="J21" s="109" t="s">
+      <c r="J21" s="106" t="s">
         <v>182</v>
       </c>
-      <c r="K21" s="116"/>
+      <c r="K21" s="112" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
@@ -2758,10 +2775,10 @@
       </c>
       <c r="H22" s="22"/>
       <c r="I22" s="91"/>
-      <c r="J22" s="109" t="s">
+      <c r="J22" s="106" t="s">
         <v>183</v>
       </c>
-      <c r="K22" s="116"/>
+      <c r="K22" s="111"/>
     </row>
     <row r="23" spans="1:11" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="72" t="s">
@@ -2785,10 +2802,10 @@
       </c>
       <c r="H23" s="74"/>
       <c r="I23" s="92"/>
-      <c r="J23" s="109" t="s">
+      <c r="J23" s="106" t="s">
         <v>183</v>
       </c>
-      <c r="K23" s="116"/>
+      <c r="K23" s="111"/>
     </row>
     <row r="24" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" s="36" t="s">
@@ -2812,10 +2829,10 @@
       </c>
       <c r="H24" s="38"/>
       <c r="I24" s="86"/>
-      <c r="J24" s="109" t="s">
+      <c r="J24" s="106" t="s">
         <v>182</v>
       </c>
-      <c r="K24" s="116"/>
+      <c r="K24" s="111"/>
     </row>
     <row r="25" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A25" s="78" t="s">
@@ -2839,10 +2856,10 @@
       </c>
       <c r="H25" s="44"/>
       <c r="I25" s="87"/>
-      <c r="J25" s="109" t="s">
+      <c r="J25" s="106" t="s">
         <v>183</v>
       </c>
-      <c r="K25" s="116"/>
+      <c r="K25" s="111"/>
     </row>
     <row r="26" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A26" s="78" t="s">
@@ -2866,8 +2883,8 @@
       </c>
       <c r="H26" s="44"/>
       <c r="I26" s="87"/>
-      <c r="J26" s="110"/>
-      <c r="K26" s="116"/>
+      <c r="J26" s="107"/>
+      <c r="K26" s="111"/>
     </row>
     <row r="27" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A27" s="78" t="s">
@@ -2891,8 +2908,8 @@
       </c>
       <c r="H27" s="44"/>
       <c r="I27" s="87"/>
-      <c r="J27" s="110"/>
-      <c r="K27" s="116"/>
+      <c r="J27" s="107"/>
+      <c r="K27" s="111"/>
     </row>
     <row r="28" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A28" s="78" t="s">
@@ -2916,8 +2933,8 @@
       </c>
       <c r="H28" s="44"/>
       <c r="I28" s="87"/>
-      <c r="J28" s="110"/>
-      <c r="K28" s="116"/>
+      <c r="J28" s="107"/>
+      <c r="K28" s="111"/>
     </row>
     <row r="29" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="78" t="s">
@@ -2941,8 +2958,8 @@
       </c>
       <c r="H29" s="44"/>
       <c r="I29" s="87"/>
-      <c r="J29" s="110"/>
-      <c r="K29" s="116"/>
+      <c r="J29" s="107"/>
+      <c r="K29" s="111"/>
     </row>
     <row r="30" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A30" s="78" t="s">
@@ -2966,8 +2983,8 @@
       </c>
       <c r="H30" s="44"/>
       <c r="I30" s="87"/>
-      <c r="J30" s="110"/>
-      <c r="K30" s="116"/>
+      <c r="J30" s="107"/>
+      <c r="K30" s="111"/>
     </row>
     <row r="31" spans="1:11" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="80" t="s">
@@ -2993,8 +3010,8 @@
       <c r="I31" s="93" t="s">
         <v>180</v>
       </c>
-      <c r="J31" s="110"/>
-      <c r="K31" s="116"/>
+      <c r="J31" s="107"/>
+      <c r="K31" s="111"/>
     </row>
     <row r="32" spans="1:11" ht="216" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
@@ -3020,10 +3037,10 @@
       <c r="I32" s="94" t="s">
         <v>131</v>
       </c>
-      <c r="J32" s="109" t="s">
+      <c r="J32" s="106" t="s">
         <v>182</v>
       </c>
-      <c r="K32" s="116"/>
+      <c r="K32" s="111"/>
     </row>
     <row r="33" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A33" s="71" t="s">
@@ -3049,10 +3066,10 @@
       <c r="I33" s="95" t="s">
         <v>131</v>
       </c>
-      <c r="J33" s="109" t="s">
+      <c r="J33" s="106" t="s">
         <v>182</v>
       </c>
-      <c r="K33" s="116"/>
+      <c r="K33" s="111"/>
     </row>
     <row r="34" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A34" s="71" t="s">
@@ -3076,10 +3093,10 @@
       </c>
       <c r="H34" s="32"/>
       <c r="I34" s="95"/>
-      <c r="J34" s="109" t="s">
+      <c r="J34" s="106" t="s">
         <v>183</v>
       </c>
-      <c r="K34" s="116"/>
+      <c r="K34" s="111"/>
     </row>
     <row r="35" spans="1:11" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="79" t="s">
@@ -3103,10 +3120,10 @@
       </c>
       <c r="H35" s="34"/>
       <c r="I35" s="96"/>
-      <c r="J35" s="109" t="s">
+      <c r="J35" s="106" t="s">
         <v>182</v>
       </c>
-      <c r="K35" s="116"/>
+      <c r="K35" s="111"/>
     </row>
     <row r="36" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="36" t="s">
@@ -3130,10 +3147,10 @@
       </c>
       <c r="H36" s="38"/>
       <c r="I36" s="86"/>
-      <c r="J36" s="109" t="s">
+      <c r="J36" s="106" t="s">
         <v>182</v>
       </c>
-      <c r="K36" s="116"/>
+      <c r="K36" s="111"/>
     </row>
     <row r="37" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="78" t="s">
@@ -3157,10 +3174,10 @@
       </c>
       <c r="H37" s="44"/>
       <c r="I37" s="87"/>
-      <c r="J37" s="109" t="s">
+      <c r="J37" s="106" t="s">
         <v>183</v>
       </c>
-      <c r="K37" s="116"/>
+      <c r="K37" s="111"/>
     </row>
     <row r="38" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="76" t="s">
@@ -3184,10 +3201,10 @@
       </c>
       <c r="H38" s="47"/>
       <c r="I38" s="90"/>
-      <c r="J38" s="109" t="s">
+      <c r="J38" s="106" t="s">
         <v>183</v>
       </c>
-      <c r="K38" s="116"/>
+      <c r="K38" s="111"/>
     </row>
     <row r="39" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="40" t="s">
@@ -3213,10 +3230,10 @@
       <c r="I39" s="97" t="s">
         <v>176</v>
       </c>
-      <c r="J39" s="109" t="s">
+      <c r="J39" s="106" t="s">
         <v>183</v>
       </c>
-      <c r="K39" s="116"/>
+      <c r="K39" s="111"/>
     </row>
     <row r="40" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
@@ -3240,10 +3257,10 @@
       </c>
       <c r="H40" s="18"/>
       <c r="I40" s="84"/>
-      <c r="J40" s="111" t="s">
+      <c r="J40" s="121" t="s">
         <v>182</v>
       </c>
-      <c r="K40" s="116"/>
+      <c r="K40" s="111"/>
     </row>
     <row r="41" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
@@ -3269,8 +3286,8 @@
       <c r="I41" s="98" t="s">
         <v>163</v>
       </c>
-      <c r="J41" s="112"/>
-      <c r="K41" s="116"/>
+      <c r="J41" s="122"/>
+      <c r="K41" s="111"/>
     </row>
     <row r="42" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
@@ -3296,8 +3313,8 @@
       <c r="I42" s="98" t="s">
         <v>163</v>
       </c>
-      <c r="J42" s="112"/>
-      <c r="K42" s="116"/>
+      <c r="J42" s="122"/>
+      <c r="K42" s="111"/>
     </row>
     <row r="43" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="24" t="s">
@@ -3321,8 +3338,8 @@
       </c>
       <c r="H43" s="26"/>
       <c r="I43" s="85"/>
-      <c r="J43" s="112"/>
-      <c r="K43" s="116"/>
+      <c r="J43" s="122"/>
+      <c r="K43" s="111"/>
     </row>
     <row r="44" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="24" t="s">
@@ -3348,8 +3365,8 @@
       <c r="I44" s="99" t="s">
         <v>174</v>
       </c>
-      <c r="J44" s="112"/>
-      <c r="K44" s="115"/>
+      <c r="J44" s="122"/>
+      <c r="K44" s="110"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="10"/>

</xml_diff>

<commit_message>
Created AboutPage & AboutTest
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E96C18-6AD9-472C-8248-F8A87D9CA13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE8DE74-BF92-4AC7-A13F-ED37A4740987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="188">
   <si>
     <t>ID</t>
   </si>
@@ -886,12 +886,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1468,374 +1476,374 @@
   </cellStyleXfs>
   <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2120,8 +2128,8 @@
   <dimension ref="A1:K176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2135,8 +2143,8 @@
     <col min="7" max="7" width="60.44140625" style="14" customWidth="1"/>
     <col min="8" max="8" width="28.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" style="82" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.44140625" style="82" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" style="81" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" style="81" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
@@ -2165,13 +2173,13 @@
       <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="83" t="s">
+      <c r="I1" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="101" t="s">
+      <c r="J1" s="100" t="s">
         <v>181</v>
       </c>
-      <c r="K1" s="108" t="s">
+      <c r="K1" s="107" t="s">
         <v>184</v>
       </c>
     </row>
@@ -2196,11 +2204,11 @@
         <v>16</v>
       </c>
       <c r="H2" s="18"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="102" t="s">
+      <c r="I2" s="83"/>
+      <c r="J2" s="101" t="s">
         <v>183</v>
       </c>
-      <c r="K2" s="109"/>
+      <c r="K2" s="108"/>
     </row>
     <row r="3" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
@@ -2223,14 +2231,14 @@
         <v>19</v>
       </c>
       <c r="H3" s="26"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="103" t="s">
+      <c r="I3" s="84"/>
+      <c r="J3" s="102" t="s">
         <v>183</v>
       </c>
-      <c r="K3" s="110"/>
+      <c r="K3" s="109"/>
     </row>
     <row r="4" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="99" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="53" t="s">
@@ -2252,11 +2260,11 @@
       <c r="H4" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="86"/>
+      <c r="I4" s="85"/>
       <c r="J4" s="118" t="s">
         <v>182</v>
       </c>
-      <c r="K4" s="112" t="s">
+      <c r="K4" s="111" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2283,11 +2291,11 @@
       <c r="H5" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="87" t="s">
+      <c r="I5" s="86" t="s">
         <v>27</v>
       </c>
       <c r="J5" s="119"/>
-      <c r="K5" s="111"/>
+      <c r="K5" s="110"/>
     </row>
     <row r="6" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="54" t="s">
@@ -2306,17 +2314,17 @@
       <c r="F6" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="117" t="s">
+      <c r="G6" s="116" t="s">
         <v>36</v>
       </c>
       <c r="H6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="87" t="s">
+      <c r="I6" s="86" t="s">
         <v>27</v>
       </c>
       <c r="J6" s="119"/>
-      <c r="K6" s="112" t="s">
+      <c r="K6" s="111" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2343,11 +2351,11 @@
       <c r="H7" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="87" t="s">
+      <c r="I7" s="86" t="s">
         <v>27</v>
       </c>
       <c r="J7" s="119"/>
-      <c r="K7" s="112" t="s">
+      <c r="K7" s="111" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2374,9 +2382,9 @@
       <c r="H8" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="87"/>
+      <c r="I8" s="86"/>
       <c r="J8" s="119"/>
-      <c r="K8" s="112" t="s">
+      <c r="K8" s="111" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2403,9 +2411,9 @@
       <c r="H9" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="87"/>
+      <c r="I9" s="86"/>
       <c r="J9" s="119"/>
-      <c r="K9" s="112" t="s">
+      <c r="K9" s="111" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2432,11 +2440,11 @@
       <c r="H10" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="87" t="s">
+      <c r="I10" s="86" t="s">
         <v>27</v>
       </c>
       <c r="J10" s="119"/>
-      <c r="K10" s="111"/>
+      <c r="K10" s="110"/>
     </row>
     <row r="11" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="57" t="s">
@@ -2461,9 +2469,9 @@
       <c r="H11" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="I11" s="88"/>
+      <c r="I11" s="87"/>
       <c r="J11" s="120"/>
-      <c r="K11" s="112" t="s">
+      <c r="K11" s="111" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2471,7 +2479,7 @@
       <c r="A12" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="114" t="s">
+      <c r="B12" s="113" t="s">
         <v>186</v>
       </c>
       <c r="C12" s="59"/>
@@ -2481,18 +2489,18 @@
       <c r="E12" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="115" t="s">
+      <c r="F12" s="114" t="s">
         <v>187</v>
       </c>
-      <c r="G12" s="116" t="s">
+      <c r="G12" s="115" t="s">
         <v>34</v>
       </c>
       <c r="H12" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="I12" s="88"/>
-      <c r="J12" s="113"/>
-      <c r="K12" s="112" t="s">
+      <c r="I12" s="87"/>
+      <c r="J12" s="112"/>
+      <c r="K12" s="111" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2519,11 +2527,11 @@
       <c r="H13" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="I13" s="84"/>
-      <c r="J13" s="102" t="s">
+      <c r="I13" s="83"/>
+      <c r="J13" s="101" t="s">
         <v>182</v>
       </c>
-      <c r="K13" s="123"/>
+      <c r="K13" s="117"/>
     </row>
     <row r="14" spans="1:11" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
@@ -2548,11 +2556,11 @@
       <c r="H14" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="I14" s="85"/>
-      <c r="J14" s="103" t="s">
+      <c r="I14" s="84"/>
+      <c r="J14" s="102" t="s">
         <v>183</v>
       </c>
-      <c r="K14" s="111"/>
+      <c r="K14" s="110"/>
     </row>
     <row r="15" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="36" t="s">
@@ -2575,11 +2583,11 @@
         <v>68</v>
       </c>
       <c r="H15" s="38"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="102" t="s">
+      <c r="I15" s="85"/>
+      <c r="J15" s="101" t="s">
         <v>182</v>
       </c>
-      <c r="K15" s="123"/>
+      <c r="K15" s="117"/>
     </row>
     <row r="16" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="40" t="s">
@@ -2602,11 +2610,11 @@
         <v>72</v>
       </c>
       <c r="H16" s="44"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="104" t="s">
+      <c r="I16" s="86"/>
+      <c r="J16" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="K16" s="112" t="s">
+      <c r="K16" s="111" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2631,13 +2639,13 @@
         <v>76</v>
       </c>
       <c r="H17" s="44"/>
-      <c r="I17" s="89" t="s">
+      <c r="I17" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="J17" s="104" t="s">
+      <c r="J17" s="103" t="s">
         <v>183</v>
       </c>
-      <c r="K17" s="111"/>
+      <c r="K17" s="110"/>
     </row>
     <row r="18" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="40" t="s">
@@ -2660,11 +2668,11 @@
         <v>81</v>
       </c>
       <c r="H18" s="44"/>
-      <c r="I18" s="89"/>
-      <c r="J18" s="104" t="s">
+      <c r="I18" s="88"/>
+      <c r="J18" s="103" t="s">
         <v>183</v>
       </c>
-      <c r="K18" s="111"/>
+      <c r="K18" s="110"/>
     </row>
     <row r="19" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="45" t="s">
@@ -2687,11 +2695,11 @@
         <v>85</v>
       </c>
       <c r="H19" s="47"/>
-      <c r="I19" s="90"/>
-      <c r="J19" s="103" t="s">
+      <c r="I19" s="89"/>
+      <c r="J19" s="102" t="s">
         <v>182</v>
       </c>
-      <c r="K19" s="112" t="s">
+      <c r="K19" s="111" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2716,11 +2724,11 @@
         <v>72</v>
       </c>
       <c r="H20" s="18"/>
-      <c r="I20" s="84"/>
-      <c r="J20" s="105" t="s">
+      <c r="I20" s="83"/>
+      <c r="J20" s="104" t="s">
         <v>182</v>
       </c>
-      <c r="K20" s="112" t="s">
+      <c r="K20" s="111" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2745,11 +2753,11 @@
         <v>72</v>
       </c>
       <c r="H21" s="22"/>
-      <c r="I21" s="91"/>
-      <c r="J21" s="106" t="s">
+      <c r="I21" s="90"/>
+      <c r="J21" s="105" t="s">
         <v>182</v>
       </c>
-      <c r="K21" s="112" t="s">
+      <c r="K21" s="111" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2774,11 +2782,11 @@
         <v>94</v>
       </c>
       <c r="H22" s="22"/>
-      <c r="I22" s="91"/>
-      <c r="J22" s="106" t="s">
+      <c r="I22" s="90"/>
+      <c r="J22" s="105" t="s">
         <v>183</v>
       </c>
-      <c r="K22" s="111"/>
+      <c r="K22" s="110"/>
     </row>
     <row r="23" spans="1:11" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="72" t="s">
@@ -2801,11 +2809,11 @@
         <v>98</v>
       </c>
       <c r="H23" s="74"/>
-      <c r="I23" s="92"/>
-      <c r="J23" s="106" t="s">
+      <c r="I23" s="91"/>
+      <c r="J23" s="105" t="s">
         <v>183</v>
       </c>
-      <c r="K23" s="111"/>
+      <c r="K23" s="110"/>
     </row>
     <row r="24" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" s="36" t="s">
@@ -2828,17 +2836,17 @@
         <v>107</v>
       </c>
       <c r="H24" s="38"/>
-      <c r="I24" s="86"/>
-      <c r="J24" s="106" t="s">
+      <c r="I24" s="85"/>
+      <c r="J24" s="105" t="s">
         <v>182</v>
       </c>
-      <c r="K24" s="111"/>
+      <c r="K24" s="110"/>
     </row>
     <row r="25" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="78" t="s">
+      <c r="A25" s="77" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="77" t="s">
+      <c r="B25" s="76" t="s">
         <v>108</v>
       </c>
       <c r="C25" s="44"/>
@@ -2855,17 +2863,17 @@
         <v>109</v>
       </c>
       <c r="H25" s="44"/>
-      <c r="I25" s="87"/>
-      <c r="J25" s="106" t="s">
+      <c r="I25" s="86"/>
+      <c r="J25" s="105" t="s">
         <v>183</v>
       </c>
-      <c r="K25" s="111"/>
+      <c r="K25" s="110"/>
     </row>
     <row r="26" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="78" t="s">
+      <c r="A26" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="77" t="s">
+      <c r="B26" s="76" t="s">
         <v>110</v>
       </c>
       <c r="C26" s="44"/>
@@ -2882,12 +2890,12 @@
         <v>114</v>
       </c>
       <c r="H26" s="44"/>
-      <c r="I26" s="87"/>
-      <c r="J26" s="107"/>
-      <c r="K26" s="111"/>
+      <c r="I26" s="86"/>
+      <c r="J26" s="106"/>
+      <c r="K26" s="110"/>
     </row>
     <row r="27" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="77" t="s">
         <v>102</v>
       </c>
       <c r="B27" s="68" t="s">
@@ -2907,12 +2915,12 @@
         <v>117</v>
       </c>
       <c r="H27" s="44"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="107"/>
-      <c r="K27" s="111"/>
+      <c r="I27" s="86"/>
+      <c r="J27" s="106"/>
+      <c r="K27" s="110"/>
     </row>
     <row r="28" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="78" t="s">
+      <c r="A28" s="77" t="s">
         <v>103</v>
       </c>
       <c r="B28" s="68" t="s">
@@ -2932,12 +2940,12 @@
         <v>120</v>
       </c>
       <c r="H28" s="44"/>
-      <c r="I28" s="87"/>
-      <c r="J28" s="107"/>
-      <c r="K28" s="111"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="106"/>
+      <c r="K28" s="110"/>
     </row>
     <row r="29" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="78" t="s">
+      <c r="A29" s="77" t="s">
         <v>104</v>
       </c>
       <c r="B29" s="68" t="s">
@@ -2957,12 +2965,12 @@
         <v>122</v>
       </c>
       <c r="H29" s="44"/>
-      <c r="I29" s="87"/>
-      <c r="J29" s="107"/>
-      <c r="K29" s="111"/>
+      <c r="I29" s="86"/>
+      <c r="J29" s="106"/>
+      <c r="K29" s="110"/>
     </row>
     <row r="30" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="78" t="s">
+      <c r="A30" s="77" t="s">
         <v>105</v>
       </c>
       <c r="B30" s="68" t="s">
@@ -2982,15 +2990,15 @@
         <v>126</v>
       </c>
       <c r="H30" s="44"/>
-      <c r="I30" s="87"/>
-      <c r="J30" s="107"/>
-      <c r="K30" s="111"/>
+      <c r="I30" s="86"/>
+      <c r="J30" s="106"/>
+      <c r="K30" s="110"/>
     </row>
     <row r="31" spans="1:11" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="80" t="s">
+      <c r="A31" s="79" t="s">
         <v>178</v>
       </c>
-      <c r="B31" s="81" t="s">
+      <c r="B31" s="80" t="s">
         <v>179</v>
       </c>
       <c r="C31" s="44"/>
@@ -3007,11 +3015,11 @@
         <v>126</v>
       </c>
       <c r="H31" s="44"/>
-      <c r="I31" s="93" t="s">
+      <c r="I31" s="92" t="s">
         <v>180</v>
       </c>
-      <c r="J31" s="107"/>
-      <c r="K31" s="111"/>
+      <c r="J31" s="106"/>
+      <c r="K31" s="110"/>
     </row>
     <row r="32" spans="1:11" ht="216" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
@@ -3034,13 +3042,13 @@
         <v>130</v>
       </c>
       <c r="H32" s="30"/>
-      <c r="I32" s="94" t="s">
+      <c r="I32" s="93" t="s">
         <v>131</v>
       </c>
-      <c r="J32" s="106" t="s">
+      <c r="J32" s="105" t="s">
         <v>182</v>
       </c>
-      <c r="K32" s="111"/>
+      <c r="K32" s="110"/>
     </row>
     <row r="33" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A33" s="71" t="s">
@@ -3063,13 +3071,13 @@
         <v>136</v>
       </c>
       <c r="H33" s="32"/>
-      <c r="I33" s="95" t="s">
+      <c r="I33" s="94" t="s">
         <v>131</v>
       </c>
-      <c r="J33" s="106" t="s">
+      <c r="J33" s="105" t="s">
         <v>182</v>
       </c>
-      <c r="K33" s="111"/>
+      <c r="K33" s="110"/>
     </row>
     <row r="34" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A34" s="71" t="s">
@@ -3092,14 +3100,14 @@
         <v>140</v>
       </c>
       <c r="H34" s="32"/>
-      <c r="I34" s="95"/>
-      <c r="J34" s="106" t="s">
+      <c r="I34" s="94"/>
+      <c r="J34" s="105" t="s">
         <v>183</v>
       </c>
-      <c r="K34" s="111"/>
+      <c r="K34" s="110"/>
     </row>
     <row r="35" spans="1:11" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="79" t="s">
+      <c r="A35" s="78" t="s">
         <v>141</v>
       </c>
       <c r="B35" s="33" t="s">
@@ -3119,11 +3127,11 @@
         <v>143</v>
       </c>
       <c r="H35" s="34"/>
-      <c r="I35" s="96"/>
-      <c r="J35" s="106" t="s">
+      <c r="I35" s="95"/>
+      <c r="J35" s="105" t="s">
         <v>182</v>
       </c>
-      <c r="K35" s="111"/>
+      <c r="K35" s="110"/>
     </row>
     <row r="36" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="36" t="s">
@@ -3146,14 +3154,16 @@
         <v>147</v>
       </c>
       <c r="H36" s="38"/>
-      <c r="I36" s="86"/>
-      <c r="J36" s="106" t="s">
+      <c r="I36" s="85"/>
+      <c r="J36" s="105" t="s">
         <v>182</v>
       </c>
-      <c r="K36" s="111"/>
+      <c r="K36" s="111" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="37" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="78" t="s">
+      <c r="A37" s="77" t="s">
         <v>148</v>
       </c>
       <c r="B37" s="68" t="s">
@@ -3173,14 +3183,14 @@
         <v>151</v>
       </c>
       <c r="H37" s="44"/>
-      <c r="I37" s="87"/>
-      <c r="J37" s="106" t="s">
+      <c r="I37" s="86"/>
+      <c r="J37" s="105" t="s">
         <v>183</v>
       </c>
-      <c r="K37" s="111"/>
+      <c r="K37" s="110"/>
     </row>
     <row r="38" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="76" t="s">
+      <c r="A38" s="123" t="s">
         <v>152</v>
       </c>
       <c r="B38" s="68" t="s">
@@ -3200,11 +3210,11 @@
         <v>155</v>
       </c>
       <c r="H38" s="47"/>
-      <c r="I38" s="90"/>
-      <c r="J38" s="106" t="s">
+      <c r="I38" s="89"/>
+      <c r="J38" s="105" t="s">
         <v>183</v>
       </c>
-      <c r="K38" s="111"/>
+      <c r="K38" s="110"/>
     </row>
     <row r="39" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="40" t="s">
@@ -3227,13 +3237,13 @@
         <v>147</v>
       </c>
       <c r="H39" s="47"/>
-      <c r="I39" s="97" t="s">
+      <c r="I39" s="96" t="s">
         <v>176</v>
       </c>
-      <c r="J39" s="106" t="s">
+      <c r="J39" s="105" t="s">
         <v>183</v>
       </c>
-      <c r="K39" s="111"/>
+      <c r="K39" s="110"/>
     </row>
     <row r="40" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
@@ -3256,11 +3266,11 @@
         <v>159</v>
       </c>
       <c r="H40" s="18"/>
-      <c r="I40" s="84"/>
+      <c r="I40" s="83"/>
       <c r="J40" s="121" t="s">
         <v>182</v>
       </c>
-      <c r="K40" s="111"/>
+      <c r="K40" s="110"/>
     </row>
     <row r="41" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
@@ -3283,11 +3293,11 @@
         <v>162</v>
       </c>
       <c r="H41" s="65"/>
-      <c r="I41" s="98" t="s">
+      <c r="I41" s="97" t="s">
         <v>163</v>
       </c>
       <c r="J41" s="122"/>
-      <c r="K41" s="111"/>
+      <c r="K41" s="110"/>
     </row>
     <row r="42" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
@@ -3310,11 +3320,11 @@
         <v>167</v>
       </c>
       <c r="H42" s="65"/>
-      <c r="I42" s="98" t="s">
+      <c r="I42" s="97" t="s">
         <v>163</v>
       </c>
       <c r="J42" s="122"/>
-      <c r="K42" s="111"/>
+      <c r="K42" s="110"/>
     </row>
     <row r="43" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="24" t="s">
@@ -3337,9 +3347,9 @@
         <v>170</v>
       </c>
       <c r="H43" s="26"/>
-      <c r="I43" s="85"/>
+      <c r="I43" s="84"/>
       <c r="J43" s="122"/>
-      <c r="K43" s="111"/>
+      <c r="K43" s="110"/>
     </row>
     <row r="44" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="24" t="s">
@@ -3362,11 +3372,11 @@
         <v>170</v>
       </c>
       <c r="H44" s="26"/>
-      <c r="I44" s="99" t="s">
+      <c r="I44" s="98" t="s">
         <v>174</v>
       </c>
       <c r="J44" s="122"/>
-      <c r="K44" s="110"/>
+      <c r="K44" s="109"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="10"/>

</xml_diff>

<commit_message>
Edited tests in AboutTest, LoginTest
Добавил все тесты на странице About. Починил тест с открытием уже залогиненного приложения. Вынес все переменные туда где они должны быть
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE8DE74-BF92-4AC7-A13F-ED37A4740987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165322A6-706A-454B-9DAE-3D7FF94CE6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="191">
   <si>
     <t>ID</t>
   </si>
@@ -795,9 +795,6 @@
 3. Открывается браузер на странице с политиками конфиденциальности</t>
   </si>
   <si>
-    <t>Веб страница не открывается</t>
-  </si>
-  <si>
     <t>ABOUTPAGE_2</t>
   </si>
   <si>
@@ -881,17 +878,45 @@
 4. Нажать кнопку "Войти"
 5. Нажать на значок человечка =&gt; Выйти</t>
   </si>
+  <si>
+    <t>Отображение пользовательских соглашений</t>
+  </si>
+  <si>
+    <t>Проверка правилной передачи ссылки по внешнее приложение</t>
+  </si>
+  <si>
+    <t>Ссылка заканчивается /</t>
+  </si>
+  <si>
+    <t>Ссылка заканчивается / - отсутствует</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1474,166 +1499,238 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1641,209 +1738,140 @@
     <xf numFmtId="49" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2128,8 +2156,8 @@
   <dimension ref="A1:K176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2143,8 +2171,8 @@
     <col min="7" max="7" width="60.44140625" style="14" customWidth="1"/>
     <col min="8" max="8" width="28.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" style="81" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.44140625" style="81" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" style="80" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" style="80" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
@@ -2173,14 +2201,14 @@
       <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="82" t="s">
+      <c r="I1" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="100" t="s">
-        <v>181</v>
-      </c>
-      <c r="K1" s="107" t="s">
-        <v>184</v>
+      <c r="J1" s="98" t="s">
+        <v>180</v>
+      </c>
+      <c r="K1" s="105" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -2204,11 +2232,11 @@
         <v>16</v>
       </c>
       <c r="H2" s="18"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="101" t="s">
-        <v>183</v>
-      </c>
-      <c r="K2" s="108"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="99" t="s">
+        <v>182</v>
+      </c>
+      <c r="K2" s="106"/>
     </row>
     <row r="3" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
@@ -2231,14 +2259,14 @@
         <v>19</v>
       </c>
       <c r="H3" s="26"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="102" t="s">
-        <v>183</v>
-      </c>
-      <c r="K3" s="109"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="100" t="s">
+        <v>182</v>
+      </c>
+      <c r="K3" s="107"/>
     </row>
     <row r="4" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="97" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="53" t="s">
@@ -2260,12 +2288,12 @@
       <c r="H4" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="85"/>
+      <c r="I4" s="84"/>
       <c r="J4" s="118" t="s">
-        <v>182</v>
-      </c>
-      <c r="K4" s="111" t="s">
-        <v>185</v>
+        <v>181</v>
+      </c>
+      <c r="K4" s="109" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -2291,11 +2319,11 @@
       <c r="H5" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="86" t="s">
+      <c r="I5" s="85" t="s">
         <v>27</v>
       </c>
       <c r="J5" s="119"/>
-      <c r="K5" s="110"/>
+      <c r="K5" s="108"/>
     </row>
     <row r="6" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="54" t="s">
@@ -2314,18 +2342,18 @@
       <c r="F6" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="116" t="s">
+      <c r="G6" s="114" t="s">
         <v>36</v>
       </c>
       <c r="H6" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="86" t="s">
+      <c r="I6" s="85" t="s">
         <v>27</v>
       </c>
       <c r="J6" s="119"/>
-      <c r="K6" s="111" t="s">
-        <v>185</v>
+      <c r="K6" s="109" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -2351,12 +2379,12 @@
       <c r="H7" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="86" t="s">
+      <c r="I7" s="85" t="s">
         <v>27</v>
       </c>
       <c r="J7" s="119"/>
-      <c r="K7" s="111" t="s">
-        <v>185</v>
+      <c r="K7" s="109" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -2382,10 +2410,10 @@
       <c r="H8" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="86"/>
+      <c r="I8" s="85"/>
       <c r="J8" s="119"/>
-      <c r="K8" s="111" t="s">
-        <v>185</v>
+      <c r="K8" s="109" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -2411,10 +2439,10 @@
       <c r="H9" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="86"/>
+      <c r="I9" s="85"/>
       <c r="J9" s="119"/>
-      <c r="K9" s="111" t="s">
-        <v>185</v>
+      <c r="K9" s="109" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -2440,11 +2468,11 @@
       <c r="H10" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="86" t="s">
+      <c r="I10" s="85" t="s">
         <v>27</v>
       </c>
       <c r="J10" s="119"/>
-      <c r="K10" s="110"/>
+      <c r="K10" s="108"/>
     </row>
     <row r="11" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="57" t="s">
@@ -2469,18 +2497,18 @@
       <c r="H11" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="I11" s="87"/>
+      <c r="I11" s="86"/>
       <c r="J11" s="120"/>
-      <c r="K11" s="111" t="s">
-        <v>185</v>
+      <c r="K11" s="109" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="113" t="s">
-        <v>186</v>
+      <c r="B12" s="111" t="s">
+        <v>185</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="59" t="s">
@@ -2489,19 +2517,19 @@
       <c r="E12" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="114" t="s">
-        <v>187</v>
-      </c>
-      <c r="G12" s="115" t="s">
+      <c r="F12" s="112" t="s">
+        <v>186</v>
+      </c>
+      <c r="G12" s="113" t="s">
         <v>34</v>
       </c>
       <c r="H12" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="I12" s="87"/>
-      <c r="J12" s="112"/>
-      <c r="K12" s="111" t="s">
-        <v>185</v>
+      <c r="I12" s="86"/>
+      <c r="J12" s="110"/>
+      <c r="K12" s="109" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
@@ -2527,11 +2555,11 @@
       <c r="H13" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="I13" s="83"/>
-      <c r="J13" s="101" t="s">
-        <v>182</v>
-      </c>
-      <c r="K13" s="117"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="99" t="s">
+        <v>181</v>
+      </c>
+      <c r="K13" s="115"/>
     </row>
     <row r="14" spans="1:11" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
@@ -2556,11 +2584,11 @@
       <c r="H14" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="I14" s="84"/>
-      <c r="J14" s="102" t="s">
-        <v>183</v>
-      </c>
-      <c r="K14" s="110"/>
+      <c r="I14" s="83"/>
+      <c r="J14" s="100" t="s">
+        <v>182</v>
+      </c>
+      <c r="K14" s="108"/>
     </row>
     <row r="15" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="36" t="s">
@@ -2583,11 +2611,11 @@
         <v>68</v>
       </c>
       <c r="H15" s="38"/>
-      <c r="I15" s="85"/>
-      <c r="J15" s="101" t="s">
-        <v>182</v>
-      </c>
-      <c r="K15" s="117"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="99" t="s">
+        <v>181</v>
+      </c>
+      <c r="K15" s="115"/>
     </row>
     <row r="16" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="40" t="s">
@@ -2610,12 +2638,12 @@
         <v>72</v>
       </c>
       <c r="H16" s="44"/>
-      <c r="I16" s="86"/>
-      <c r="J16" s="103" t="s">
-        <v>182</v>
-      </c>
-      <c r="K16" s="111" t="s">
-        <v>185</v>
+      <c r="I16" s="85"/>
+      <c r="J16" s="101" t="s">
+        <v>181</v>
+      </c>
+      <c r="K16" s="109" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -2639,13 +2667,13 @@
         <v>76</v>
       </c>
       <c r="H17" s="44"/>
-      <c r="I17" s="88" t="s">
+      <c r="I17" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="J17" s="103" t="s">
-        <v>183</v>
-      </c>
-      <c r="K17" s="110"/>
+      <c r="J17" s="101" t="s">
+        <v>182</v>
+      </c>
+      <c r="K17" s="108"/>
     </row>
     <row r="18" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="40" t="s">
@@ -2668,11 +2696,11 @@
         <v>81</v>
       </c>
       <c r="H18" s="44"/>
-      <c r="I18" s="88"/>
-      <c r="J18" s="103" t="s">
-        <v>183</v>
-      </c>
-      <c r="K18" s="110"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="101" t="s">
+        <v>182</v>
+      </c>
+      <c r="K18" s="108"/>
     </row>
     <row r="19" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="45" t="s">
@@ -2695,12 +2723,12 @@
         <v>85</v>
       </c>
       <c r="H19" s="47"/>
-      <c r="I19" s="89"/>
-      <c r="J19" s="102" t="s">
-        <v>182</v>
-      </c>
-      <c r="K19" s="111" t="s">
-        <v>185</v>
+      <c r="I19" s="88"/>
+      <c r="J19" s="100" t="s">
+        <v>181</v>
+      </c>
+      <c r="K19" s="109" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -2724,12 +2752,12 @@
         <v>72</v>
       </c>
       <c r="H20" s="18"/>
-      <c r="I20" s="83"/>
-      <c r="J20" s="104" t="s">
-        <v>182</v>
-      </c>
-      <c r="K20" s="111" t="s">
-        <v>185</v>
+      <c r="I20" s="82"/>
+      <c r="J20" s="102" t="s">
+        <v>181</v>
+      </c>
+      <c r="K20" s="109" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -2753,12 +2781,12 @@
         <v>72</v>
       </c>
       <c r="H21" s="22"/>
-      <c r="I21" s="90"/>
-      <c r="J21" s="105" t="s">
-        <v>182</v>
-      </c>
-      <c r="K21" s="111" t="s">
-        <v>185</v>
+      <c r="I21" s="89"/>
+      <c r="J21" s="103" t="s">
+        <v>181</v>
+      </c>
+      <c r="K21" s="109" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
@@ -2782,44 +2810,44 @@
         <v>94</v>
       </c>
       <c r="H22" s="22"/>
-      <c r="I22" s="90"/>
-      <c r="J22" s="105" t="s">
-        <v>183</v>
-      </c>
-      <c r="K22" s="110"/>
+      <c r="I22" s="89"/>
+      <c r="J22" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="K22" s="108"/>
     </row>
     <row r="23" spans="1:11" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="72" t="s">
+      <c r="A23" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74" t="s">
+      <c r="C23" s="73"/>
+      <c r="D23" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="75" t="s">
+      <c r="E23" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="75" t="s">
+      <c r="F23" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="G23" s="75" t="s">
+      <c r="G23" s="74" t="s">
         <v>98</v>
       </c>
-      <c r="H23" s="74"/>
-      <c r="I23" s="91"/>
-      <c r="J23" s="105" t="s">
-        <v>183</v>
-      </c>
-      <c r="K23" s="110"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="90"/>
+      <c r="J23" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="K23" s="108"/>
     </row>
     <row r="24" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="66" t="s">
         <v>106</v>
       </c>
       <c r="C24" s="38"/>
@@ -2836,17 +2864,17 @@
         <v>107</v>
       </c>
       <c r="H24" s="38"/>
-      <c r="I24" s="85"/>
-      <c r="J24" s="105" t="s">
-        <v>182</v>
-      </c>
-      <c r="K24" s="110"/>
+      <c r="I24" s="84"/>
+      <c r="J24" s="103" t="s">
+        <v>181</v>
+      </c>
+      <c r="K24" s="108"/>
     </row>
     <row r="25" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="76" t="s">
+      <c r="B25" s="75" t="s">
         <v>108</v>
       </c>
       <c r="C25" s="44"/>
@@ -2863,17 +2891,17 @@
         <v>109</v>
       </c>
       <c r="H25" s="44"/>
-      <c r="I25" s="86"/>
-      <c r="J25" s="105" t="s">
-        <v>183</v>
-      </c>
-      <c r="K25" s="110"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="K25" s="108"/>
     </row>
     <row r="26" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="77" t="s">
+      <c r="A26" s="76" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="75" t="s">
         <v>110</v>
       </c>
       <c r="C26" s="44"/>
@@ -2890,15 +2918,15 @@
         <v>114</v>
       </c>
       <c r="H26" s="44"/>
-      <c r="I26" s="86"/>
-      <c r="J26" s="106"/>
-      <c r="K26" s="110"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="104"/>
+      <c r="K26" s="108"/>
     </row>
     <row r="27" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="76" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="67" t="s">
         <v>115</v>
       </c>
       <c r="C27" s="44"/>
@@ -2915,15 +2943,15 @@
         <v>117</v>
       </c>
       <c r="H27" s="44"/>
-      <c r="I27" s="86"/>
-      <c r="J27" s="106"/>
-      <c r="K27" s="110"/>
+      <c r="I27" s="85"/>
+      <c r="J27" s="104"/>
+      <c r="K27" s="108"/>
     </row>
     <row r="28" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="77" t="s">
+      <c r="A28" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="B28" s="68" t="s">
+      <c r="B28" s="67" t="s">
         <v>118</v>
       </c>
       <c r="C28" s="44"/>
@@ -2940,15 +2968,15 @@
         <v>120</v>
       </c>
       <c r="H28" s="44"/>
-      <c r="I28" s="86"/>
-      <c r="J28" s="106"/>
-      <c r="K28" s="110"/>
+      <c r="I28" s="85"/>
+      <c r="J28" s="104"/>
+      <c r="K28" s="108"/>
     </row>
     <row r="29" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="77" t="s">
+      <c r="A29" s="76" t="s">
         <v>104</v>
       </c>
-      <c r="B29" s="68" t="s">
+      <c r="B29" s="67" t="s">
         <v>121</v>
       </c>
       <c r="C29" s="44"/>
@@ -2965,15 +2993,15 @@
         <v>122</v>
       </c>
       <c r="H29" s="44"/>
-      <c r="I29" s="86"/>
-      <c r="J29" s="106"/>
-      <c r="K29" s="110"/>
+      <c r="I29" s="85"/>
+      <c r="J29" s="104"/>
+      <c r="K29" s="108"/>
     </row>
     <row r="30" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="77" t="s">
+      <c r="A30" s="76" t="s">
         <v>105</v>
       </c>
-      <c r="B30" s="68" t="s">
+      <c r="B30" s="67" t="s">
         <v>124</v>
       </c>
       <c r="C30" s="44"/>
@@ -2990,16 +3018,16 @@
         <v>126</v>
       </c>
       <c r="H30" s="44"/>
-      <c r="I30" s="86"/>
-      <c r="J30" s="106"/>
-      <c r="K30" s="110"/>
+      <c r="I30" s="85"/>
+      <c r="J30" s="104"/>
+      <c r="K30" s="108"/>
     </row>
     <row r="31" spans="1:11" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="79" t="s">
+      <c r="A31" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" s="79" t="s">
         <v>178</v>
-      </c>
-      <c r="B31" s="80" t="s">
-        <v>179</v>
       </c>
       <c r="C31" s="44"/>
       <c r="D31" s="44" t="s">
@@ -3015,11 +3043,11 @@
         <v>126</v>
       </c>
       <c r="H31" s="44"/>
-      <c r="I31" s="92" t="s">
-        <v>180</v>
-      </c>
-      <c r="J31" s="106"/>
-      <c r="K31" s="110"/>
+      <c r="I31" s="91" t="s">
+        <v>179</v>
+      </c>
+      <c r="J31" s="104"/>
+      <c r="K31" s="108"/>
     </row>
     <row r="32" spans="1:11" ht="216" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
@@ -3042,72 +3070,72 @@
         <v>130</v>
       </c>
       <c r="H32" s="30"/>
-      <c r="I32" s="93" t="s">
+      <c r="I32" s="92" t="s">
         <v>131</v>
       </c>
-      <c r="J32" s="105" t="s">
-        <v>182</v>
-      </c>
-      <c r="K32" s="110"/>
+      <c r="J32" s="103" t="s">
+        <v>181</v>
+      </c>
+      <c r="K32" s="108"/>
     </row>
     <row r="33" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="71" t="s">
+      <c r="A33" s="70" t="s">
         <v>132</v>
       </c>
-      <c r="B33" s="69" t="s">
+      <c r="B33" s="68" t="s">
         <v>134</v>
       </c>
       <c r="C33" s="32"/>
       <c r="D33" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="70" t="s">
+      <c r="E33" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="F33" s="70" t="s">
+      <c r="F33" s="69" t="s">
         <v>135</v>
       </c>
-      <c r="G33" s="70" t="s">
+      <c r="G33" s="69" t="s">
         <v>136</v>
       </c>
       <c r="H33" s="32"/>
-      <c r="I33" s="94" t="s">
+      <c r="I33" s="93" t="s">
         <v>131</v>
       </c>
-      <c r="J33" s="105" t="s">
-        <v>182</v>
-      </c>
-      <c r="K33" s="110"/>
+      <c r="J33" s="103" t="s">
+        <v>181</v>
+      </c>
+      <c r="K33" s="108"/>
     </row>
     <row r="34" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="71" t="s">
+      <c r="A34" s="70" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="69" t="s">
+      <c r="B34" s="68" t="s">
         <v>138</v>
       </c>
       <c r="C34" s="32"/>
       <c r="D34" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E34" s="70" t="s">
+      <c r="E34" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="F34" s="70" t="s">
+      <c r="F34" s="69" t="s">
         <v>139</v>
       </c>
-      <c r="G34" s="70" t="s">
+      <c r="G34" s="69" t="s">
         <v>140</v>
       </c>
       <c r="H34" s="32"/>
-      <c r="I34" s="94"/>
-      <c r="J34" s="105" t="s">
-        <v>183</v>
-      </c>
-      <c r="K34" s="110"/>
+      <c r="I34" s="93"/>
+      <c r="J34" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="K34" s="108"/>
     </row>
     <row r="35" spans="1:11" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="78" t="s">
+      <c r="A35" s="77" t="s">
         <v>141</v>
       </c>
       <c r="B35" s="33" t="s">
@@ -3127,11 +3155,11 @@
         <v>143</v>
       </c>
       <c r="H35" s="34"/>
-      <c r="I35" s="95"/>
-      <c r="J35" s="105" t="s">
-        <v>182</v>
-      </c>
-      <c r="K35" s="110"/>
+      <c r="I35" s="94"/>
+      <c r="J35" s="103" t="s">
+        <v>181</v>
+      </c>
+      <c r="K35" s="108"/>
     </row>
     <row r="36" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="36" t="s">
@@ -3154,19 +3182,19 @@
         <v>147</v>
       </c>
       <c r="H36" s="38"/>
-      <c r="I36" s="85"/>
-      <c r="J36" s="105" t="s">
-        <v>182</v>
-      </c>
-      <c r="K36" s="111" t="s">
-        <v>185</v>
+      <c r="I36" s="84"/>
+      <c r="J36" s="103" t="s">
+        <v>181</v>
+      </c>
+      <c r="K36" s="109" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="77" t="s">
+      <c r="A37" s="76" t="s">
         <v>148</v>
       </c>
-      <c r="B37" s="68" t="s">
+      <c r="B37" s="67" t="s">
         <v>149</v>
       </c>
       <c r="C37" s="44"/>
@@ -3183,17 +3211,17 @@
         <v>151</v>
       </c>
       <c r="H37" s="44"/>
-      <c r="I37" s="86"/>
-      <c r="J37" s="105" t="s">
-        <v>183</v>
-      </c>
-      <c r="K37" s="110"/>
+      <c r="I37" s="85"/>
+      <c r="J37" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="K37" s="108"/>
     </row>
     <row r="38" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="123" t="s">
+      <c r="A38" s="116" t="s">
         <v>152</v>
       </c>
-      <c r="B38" s="68" t="s">
+      <c r="B38" s="67" t="s">
         <v>153</v>
       </c>
       <c r="C38" s="44"/>
@@ -3210,18 +3238,18 @@
         <v>155</v>
       </c>
       <c r="H38" s="47"/>
-      <c r="I38" s="89"/>
-      <c r="J38" s="105" t="s">
-        <v>183</v>
-      </c>
-      <c r="K38" s="110"/>
+      <c r="I38" s="88"/>
+      <c r="J38" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="K38" s="108"/>
     </row>
     <row r="39" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B39" s="41" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C39" s="42"/>
       <c r="D39" s="43" t="s">
@@ -3237,13 +3265,13 @@
         <v>147</v>
       </c>
       <c r="H39" s="47"/>
-      <c r="I39" s="96" t="s">
-        <v>176</v>
-      </c>
-      <c r="J39" s="105" t="s">
-        <v>183</v>
-      </c>
-      <c r="K39" s="110"/>
+      <c r="I39" s="95" t="s">
+        <v>175</v>
+      </c>
+      <c r="J39" s="103" t="s">
+        <v>182</v>
+      </c>
+      <c r="K39" s="108"/>
     </row>
     <row r="40" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
@@ -3266,17 +3294,19 @@
         <v>159</v>
       </c>
       <c r="H40" s="18"/>
-      <c r="I40" s="83"/>
+      <c r="I40" s="82"/>
       <c r="J40" s="121" t="s">
-        <v>182</v>
-      </c>
-      <c r="K40" s="110"/>
+        <v>181</v>
+      </c>
+      <c r="K40" s="109" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="41" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="B41" s="66" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" s="65" t="s">
         <v>160</v>
       </c>
       <c r="C41" s="22"/>
@@ -3292,19 +3322,23 @@
       <c r="G41" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="H41" s="65"/>
-      <c r="I41" s="97" t="s">
-        <v>163</v>
+      <c r="H41" s="123" t="s">
+        <v>188</v>
+      </c>
+      <c r="I41" s="123" t="s">
+        <v>189</v>
       </c>
       <c r="J41" s="122"/>
-      <c r="K41" s="110"/>
+      <c r="K41" s="109" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="42" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="B42" s="66" t="s">
-        <v>160</v>
+        <v>164</v>
+      </c>
+      <c r="B42" s="117" t="s">
+        <v>187</v>
       </c>
       <c r="C42" s="22"/>
       <c r="D42" s="23" t="s">
@@ -3314,24 +3348,28 @@
         <v>66</v>
       </c>
       <c r="F42" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="G42" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="G42" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="H42" s="65"/>
-      <c r="I42" s="97" t="s">
-        <v>163</v>
+      <c r="H42" s="123" t="s">
+        <v>188</v>
+      </c>
+      <c r="I42" s="123" t="s">
+        <v>190</v>
       </c>
       <c r="J42" s="122"/>
-      <c r="K42" s="110"/>
+      <c r="K42" s="109" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="43" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C43" s="26"/>
       <c r="D43" s="27" t="s">
@@ -3341,22 +3379,24 @@
         <v>66</v>
       </c>
       <c r="F43" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="G43" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="G43" s="27" t="s">
-        <v>170</v>
-      </c>
       <c r="H43" s="26"/>
-      <c r="I43" s="84"/>
+      <c r="I43" s="83"/>
       <c r="J43" s="122"/>
-      <c r="K43" s="110"/>
+      <c r="K43" s="109" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="44" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" s="25" t="s">
         <v>172</v>
-      </c>
-      <c r="B44" s="25" t="s">
-        <v>173</v>
       </c>
       <c r="C44" s="26"/>
       <c r="D44" s="27" t="s">
@@ -3366,17 +3406,17 @@
         <v>66</v>
       </c>
       <c r="F44" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="G44" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="G44" s="27" t="s">
-        <v>170</v>
-      </c>
       <c r="H44" s="26"/>
-      <c r="I44" s="98" t="s">
-        <v>174</v>
+      <c r="I44" s="96" t="s">
+        <v>173</v>
       </c>
       <c r="J44" s="122"/>
-      <c r="K44" s="109"/>
+      <c r="K44" s="124"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="10"/>

</xml_diff>

<commit_message>
Edded NewsTest, optimization LoginTest, AboutTest
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165322A6-706A-454B-9DAE-3D7FF94CE6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E298C5CE-0B68-4A4B-B55F-4B20B3FAC662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="191">
   <si>
     <t>ID</t>
   </si>
@@ -1852,6 +1852,12 @@
     <xf numFmtId="49" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1865,12 +1871,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2156,8 +2156,8 @@
   <dimension ref="A1:K176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2289,7 +2289,7 @@
         <v>24</v>
       </c>
       <c r="I4" s="84"/>
-      <c r="J4" s="118" t="s">
+      <c r="J4" s="120" t="s">
         <v>181</v>
       </c>
       <c r="K4" s="109" t="s">
@@ -2322,7 +2322,7 @@
       <c r="I5" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="119"/>
+      <c r="J5" s="121"/>
       <c r="K5" s="108"/>
     </row>
     <row r="6" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -2351,7 +2351,7 @@
       <c r="I6" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="119"/>
+      <c r="J6" s="121"/>
       <c r="K6" s="109" t="s">
         <v>184</v>
       </c>
@@ -2382,7 +2382,7 @@
       <c r="I7" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="119"/>
+      <c r="J7" s="121"/>
       <c r="K7" s="109" t="s">
         <v>184</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>24</v>
       </c>
       <c r="I8" s="85"/>
-      <c r="J8" s="119"/>
+      <c r="J8" s="121"/>
       <c r="K8" s="109" t="s">
         <v>184</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>24</v>
       </c>
       <c r="I9" s="85"/>
-      <c r="J9" s="119"/>
+      <c r="J9" s="121"/>
       <c r="K9" s="109" t="s">
         <v>184</v>
       </c>
@@ -2471,7 +2471,7 @@
       <c r="I10" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="119"/>
+      <c r="J10" s="121"/>
       <c r="K10" s="108"/>
     </row>
     <row r="11" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
@@ -2498,7 +2498,7 @@
         <v>53</v>
       </c>
       <c r="I11" s="86"/>
-      <c r="J11" s="120"/>
+      <c r="J11" s="122"/>
       <c r="K11" s="109" t="s">
         <v>184</v>
       </c>
@@ -3076,7 +3076,9 @@
       <c r="J32" s="103" t="s">
         <v>181</v>
       </c>
-      <c r="K32" s="108"/>
+      <c r="K32" s="109" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="33" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A33" s="70" t="s">
@@ -3295,7 +3297,7 @@
       </c>
       <c r="H40" s="18"/>
       <c r="I40" s="82"/>
-      <c r="J40" s="121" t="s">
+      <c r="J40" s="123" t="s">
         <v>181</v>
       </c>
       <c r="K40" s="109" t="s">
@@ -3322,13 +3324,13 @@
       <c r="G41" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="H41" s="123" t="s">
+      <c r="H41" s="118" t="s">
         <v>188</v>
       </c>
-      <c r="I41" s="123" t="s">
+      <c r="I41" s="118" t="s">
         <v>189</v>
       </c>
-      <c r="J41" s="122"/>
+      <c r="J41" s="124"/>
       <c r="K41" s="109" t="s">
         <v>184</v>
       </c>
@@ -3353,13 +3355,13 @@
       <c r="G42" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="H42" s="123" t="s">
+      <c r="H42" s="118" t="s">
         <v>188</v>
       </c>
-      <c r="I42" s="123" t="s">
+      <c r="I42" s="118" t="s">
         <v>190</v>
       </c>
-      <c r="J42" s="122"/>
+      <c r="J42" s="124"/>
       <c r="K42" s="109" t="s">
         <v>184</v>
       </c>
@@ -3386,7 +3388,7 @@
       </c>
       <c r="H43" s="26"/>
       <c r="I43" s="83"/>
-      <c r="J43" s="122"/>
+      <c r="J43" s="124"/>
       <c r="K43" s="109" t="s">
         <v>184</v>
       </c>
@@ -3415,8 +3417,8 @@
       <c r="I44" s="96" t="s">
         <v>173</v>
       </c>
-      <c r="J44" s="122"/>
-      <c r="K44" s="124"/>
+      <c r="J44" s="124"/>
+      <c r="K44" s="119"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="10"/>

</xml_diff>